<commit_message>
refactor to get optimal mfcc
</commit_message>
<xml_diff>
--- a/model_comparison.xlsx
+++ b/model_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\hugo-dev\esirem-dev\4a\kmutt\kmutt_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A149540-595E-49B0-9C98-4C2404550DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EE49F9-7700-40B9-BDA7-91D1BAFE50B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="61">
   <si>
     <t>Model</t>
   </si>
@@ -102,6 +102,111 @@
   </si>
   <si>
     <t>Colonne10</t>
+  </si>
+  <si>
+    <t>0.9282</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.93 </t>
+  </si>
+  <si>
+    <t>0.9601</t>
+  </si>
+  <si>
+    <t>0.8581</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>0.9211</t>
+  </si>
+  <si>
+    <t>0.8206</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>0.9003</t>
+  </si>
+  <si>
+    <t>0.8868</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>0.9371</t>
+  </si>
+  <si>
+    <t>0.8882</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.9378</t>
+  </si>
+  <si>
+    <t>0.7747</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>0.66</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>0.8748</t>
+  </si>
+  <si>
+    <t>0.7748</t>
+  </si>
+  <si>
+    <t>0.77</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>0.8293</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>0.9051</t>
+  </si>
+  <si>
+    <t>0.6949</t>
+  </si>
+  <si>
+    <t>0.70</t>
+  </si>
+  <si>
+    <t>0.69</t>
+  </si>
+  <si>
+    <t>0.8304</t>
+  </si>
+  <si>
+    <t>0.6436</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>0.8020</t>
   </si>
 </sst>
 </file>
@@ -186,16 +291,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,12 +471,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{18D5B4DC-B117-4E07-AC9B-D242641D060A}" name="Tableau147" displayName="Tableau147" ref="A2:J22" totalsRowShown="0" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{18D5B4DC-B117-4E07-AC9B-D242641D060A}" name="Tableau147" displayName="Tableau147" ref="A2:J22" totalsRowShown="0" tableBorderDxfId="11">
   <autoFilter ref="A2:J22" xr:uid="{18D5B4DC-B117-4E07-AC9B-D242641D060A}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{030C74F2-9257-49D6-A09A-88D9AC93B4DF}" name="Colonne1"/>
-    <tableColumn id="2" xr3:uid="{C98CD88B-5B93-4AA2-9CF8-5C57AAF380AF}" name="Colonne2" dataDxfId="1" dataCellStyle="Pourcentage"/>
-    <tableColumn id="3" xr3:uid="{BA3F1E5A-29B7-47E5-BC4F-912BA3280B23}" name="Colonne3" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{C98CD88B-5B93-4AA2-9CF8-5C57AAF380AF}" name="Colonne2" dataDxfId="10" dataCellStyle="Pourcentage"/>
+    <tableColumn id="3" xr3:uid="{BA3F1E5A-29B7-47E5-BC4F-912BA3280B23}" name="Colonne3" dataDxfId="9"/>
     <tableColumn id="4" xr3:uid="{57214EBD-CC3D-4B65-9BFF-2240074956AC}" name="Colonne4"/>
     <tableColumn id="5" xr3:uid="{ED902988-0D43-4700-AF1D-8F6AE694EEC1}" name="Colonne5"/>
     <tableColumn id="6" xr3:uid="{15F23F11-6A65-40C1-988F-0AEDF11D5440}" name="Colonne6"/>
@@ -386,12 +490,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{80A47E3C-DE24-472C-836D-A201A524EC36}" name="Tableau146" displayName="Tableau146" ref="A2:J22" totalsRowShown="0" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{80A47E3C-DE24-472C-836D-A201A524EC36}" name="Tableau146" displayName="Tableau146" ref="A2:J22" totalsRowShown="0" tableBorderDxfId="8">
   <autoFilter ref="A2:J22" xr:uid="{80A47E3C-DE24-472C-836D-A201A524EC36}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{85183294-DCA1-4EDD-B82B-31745FEEFA48}" name="Colonne1"/>
-    <tableColumn id="2" xr3:uid="{FC7FEF01-BB92-4034-B591-A1C8A9CA7B03}" name="Colonne2" dataDxfId="4" dataCellStyle="Pourcentage"/>
-    <tableColumn id="3" xr3:uid="{E0292FBF-BAA8-4BCF-A34B-3429BAD376F8}" name="Colonne3" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{FC7FEF01-BB92-4034-B591-A1C8A9CA7B03}" name="Colonne2" dataDxfId="7" dataCellStyle="Pourcentage"/>
+    <tableColumn id="3" xr3:uid="{E0292FBF-BAA8-4BCF-A34B-3429BAD376F8}" name="Colonne3" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{E2548244-747B-46A7-BF00-062775604304}" name="Colonne4"/>
     <tableColumn id="5" xr3:uid="{CAA16EFE-F787-4DE3-8B11-4BD3E7F4EBB0}" name="Colonne5"/>
     <tableColumn id="6" xr3:uid="{BF3A58CD-412D-40BB-8C52-951AA6B3D440}" name="Colonne6"/>
@@ -405,12 +509,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F3BC2774-395F-44A6-B6EE-027368CADAF9}" name="Tableau14" displayName="Tableau14" ref="A2:J22" totalsRowShown="0" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F3BC2774-395F-44A6-B6EE-027368CADAF9}" name="Tableau14" displayName="Tableau14" ref="A2:J22" totalsRowShown="0" tableBorderDxfId="5">
   <autoFilter ref="A2:J22" xr:uid="{F3BC2774-395F-44A6-B6EE-027368CADAF9}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{2CD9AD2E-2C4F-4B20-A55C-5537C29D45C3}" name="Colonne1"/>
-    <tableColumn id="2" xr3:uid="{377A8631-E1FA-427D-8001-BB4593A4E49A}" name="Colonne2" dataDxfId="10" dataCellStyle="Pourcentage"/>
-    <tableColumn id="3" xr3:uid="{174F7945-14D2-4792-935D-15923C2BE678}" name="Colonne3" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{377A8631-E1FA-427D-8001-BB4593A4E49A}" name="Colonne2" dataDxfId="4" dataCellStyle="Pourcentage"/>
+    <tableColumn id="3" xr3:uid="{174F7945-14D2-4792-935D-15923C2BE678}" name="Colonne3" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{6BDF49DA-7E7D-48EF-A9E6-E7305832FA66}" name="Colonne4"/>
     <tableColumn id="5" xr3:uid="{DD554686-30C3-4552-B85E-C0898FFF8197}" name="Colonne5"/>
     <tableColumn id="6" xr3:uid="{5CB9F6CA-D9D6-4CD5-8CA7-8232E2EA6DFA}" name="Colonne6"/>
@@ -424,12 +528,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EFE3A096-1A34-4AEB-8000-334EBA5CC401}" name="Tableau145" displayName="Tableau145" ref="A2:J22" totalsRowShown="0" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EFE3A096-1A34-4AEB-8000-334EBA5CC401}" name="Tableau145" displayName="Tableau145" ref="A2:J22" totalsRowShown="0" tableBorderDxfId="2">
   <autoFilter ref="A2:J22" xr:uid="{EFE3A096-1A34-4AEB-8000-334EBA5CC401}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4E0A6415-89C7-4312-841F-9F7406D19428}" name="Colonne1"/>
-    <tableColumn id="2" xr3:uid="{0FFA9FBB-B0A8-4F9F-A594-67E6BEF2BFF6}" name="Colonne2" dataDxfId="7" dataCellStyle="Pourcentage"/>
-    <tableColumn id="3" xr3:uid="{55B339AB-05CB-4E9A-BA5B-C89F7CCAF202}" name="Colonne3" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{0FFA9FBB-B0A8-4F9F-A594-67E6BEF2BFF6}" name="Colonne2" dataDxfId="1" dataCellStyle="Pourcentage"/>
+    <tableColumn id="3" xr3:uid="{55B339AB-05CB-4E9A-BA5B-C89F7CCAF202}" name="Colonne3" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{ABE66118-088A-434A-BAB6-7DD8C84EB11A}" name="Colonne4"/>
     <tableColumn id="5" xr3:uid="{B9F1E1AE-FFFA-44C0-8D44-491619E694C3}" name="Colonne5"/>
     <tableColumn id="6" xr3:uid="{F97B7B49-10AE-4BF2-89CC-574E2B4692D0}" name="Colonne6"/>
@@ -729,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -789,39 +893,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -830,30 +934,30 @@
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
+      <c r="A3">
         <v>6</v>
       </c>
       <c r="B3" s="2">
@@ -862,16 +966,9 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" s="2">
@@ -880,16 +977,9 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+      <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" s="2">
@@ -898,16 +988,9 @@
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" s="2">
@@ -916,16 +999,9 @@
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2">
@@ -934,16 +1010,9 @@
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="A8">
         <v>16</v>
       </c>
       <c r="B8" s="2">
@@ -952,16 +1021,9 @@
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+      <c r="A9">
         <v>16</v>
       </c>
       <c r="B9" s="2">
@@ -970,16 +1032,9 @@
       <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>16</v>
       </c>
       <c r="B10" s="2">
@@ -988,16 +1043,9 @@
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+      <c r="A11">
         <v>16</v>
       </c>
       <c r="B11" s="2">
@@ -1006,16 +1054,9 @@
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+      <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" s="2">
@@ -1024,16 +1065,9 @@
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+      <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" s="2">
@@ -1042,16 +1076,9 @@
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+      <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" s="2">
@@ -1060,16 +1087,9 @@
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+      <c r="A15">
         <v>6</v>
       </c>
       <c r="B15" s="2">
@@ -1078,16 +1098,9 @@
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+      <c r="A16">
         <v>6</v>
       </c>
       <c r="B16" s="2">
@@ -1096,16 +1109,9 @@
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>6</v>
       </c>
       <c r="B17" s="2">
@@ -1114,16 +1120,9 @@
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="2">
@@ -1132,16 +1131,9 @@
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" s="2">
@@ -1150,16 +1142,9 @@
       <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" s="2">
@@ -1168,16 +1153,9 @@
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>16</v>
       </c>
       <c r="B21" s="2">
@@ -1186,16 +1164,9 @@
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>16</v>
       </c>
       <c r="B22" s="2">
@@ -1204,13 +1175,6 @@
       <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1224,52 +1188,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="21.36328125" customWidth="1"/>
+    <col min="3" max="3" width="30.08984375" customWidth="1"/>
     <col min="8" max="8" width="13.08984375" customWidth="1"/>
     <col min="9" max="9" width="20.36328125" customWidth="1"/>
     <col min="10" max="10" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1278,30 +1242,30 @@
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
+      <c r="A3">
         <v>6</v>
       </c>
       <c r="B3" s="2">
@@ -1310,16 +1274,24 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" s="2">
@@ -1328,16 +1300,24 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+      <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" s="2">
@@ -1346,16 +1326,24 @@
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" s="2">
@@ -1364,16 +1352,24 @@
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2">
@@ -1382,16 +1378,24 @@
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="A8">
         <v>16</v>
       </c>
       <c r="B8" s="2">
@@ -1400,16 +1404,24 @@
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+      <c r="A9">
         <v>16</v>
       </c>
       <c r="B9" s="2">
@@ -1418,16 +1430,24 @@
       <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>16</v>
       </c>
       <c r="B10" s="2">
@@ -1436,16 +1456,24 @@
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+      <c r="A11">
         <v>16</v>
       </c>
       <c r="B11" s="2">
@@ -1454,16 +1482,24 @@
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+      <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" s="2">
@@ -1472,16 +1508,24 @@
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+      <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" s="2">
@@ -1490,16 +1534,9 @@
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+      <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" s="2">
@@ -1508,16 +1545,9 @@
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+      <c r="A15">
         <v>6</v>
       </c>
       <c r="B15" s="2">
@@ -1526,16 +1556,9 @@
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+      <c r="A16">
         <v>6</v>
       </c>
       <c r="B16" s="2">
@@ -1544,16 +1567,9 @@
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>6</v>
       </c>
       <c r="B17" s="2">
@@ -1562,16 +1578,9 @@
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="2">
@@ -1580,16 +1589,9 @@
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" s="2">
@@ -1598,16 +1600,9 @@
       <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" s="2">
@@ -1616,16 +1611,9 @@
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>16</v>
       </c>
       <c r="B21" s="2">
@@ -1634,16 +1622,9 @@
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>16</v>
       </c>
       <c r="B22" s="2">
@@ -1652,13 +1633,6 @@
       <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1685,39 +1659,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1726,30 +1700,30 @@
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
+      <c r="A3">
         <v>6</v>
       </c>
       <c r="B3" s="2">
@@ -1758,16 +1732,9 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" s="2">
@@ -1776,16 +1743,9 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+      <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" s="2">
@@ -1794,16 +1754,9 @@
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" s="2">
@@ -1812,16 +1765,9 @@
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2">
@@ -1830,16 +1776,9 @@
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="A8">
         <v>16</v>
       </c>
       <c r="B8" s="2">
@@ -1848,16 +1787,9 @@
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+      <c r="A9">
         <v>16</v>
       </c>
       <c r="B9" s="2">
@@ -1866,16 +1798,9 @@
       <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>16</v>
       </c>
       <c r="B10" s="2">
@@ -1884,16 +1809,9 @@
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+      <c r="A11">
         <v>16</v>
       </c>
       <c r="B11" s="2">
@@ -1902,16 +1820,9 @@
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+      <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" s="2">
@@ -1920,16 +1831,9 @@
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+      <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" s="2">
@@ -1938,16 +1842,9 @@
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+      <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" s="2">
@@ -1956,16 +1853,9 @@
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+      <c r="A15">
         <v>6</v>
       </c>
       <c r="B15" s="2">
@@ -1974,16 +1864,9 @@
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+      <c r="A16">
         <v>6</v>
       </c>
       <c r="B16" s="2">
@@ -1992,16 +1875,9 @@
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>6</v>
       </c>
       <c r="B17" s="2">
@@ -2010,16 +1886,9 @@
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="2">
@@ -2028,16 +1897,9 @@
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" s="2">
@@ -2046,16 +1908,9 @@
       <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" s="2">
@@ -2064,16 +1919,9 @@
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>16</v>
       </c>
       <c r="B21" s="2">
@@ -2082,16 +1930,9 @@
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>16</v>
       </c>
       <c r="B22" s="2">
@@ -2100,13 +1941,6 @@
       <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2133,39 +1967,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2174,30 +2008,30 @@
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
+      <c r="A3">
         <v>6</v>
       </c>
       <c r="B3" s="2">
@@ -2206,16 +2040,9 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" s="2">
@@ -2224,16 +2051,9 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+      <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" s="2">
@@ -2242,16 +2062,9 @@
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" s="2">
@@ -2260,16 +2073,9 @@
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2">
@@ -2278,16 +2084,9 @@
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="A8">
         <v>16</v>
       </c>
       <c r="B8" s="2">
@@ -2296,16 +2095,9 @@
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+      <c r="A9">
         <v>16</v>
       </c>
       <c r="B9" s="2">
@@ -2314,16 +2106,9 @@
       <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>16</v>
       </c>
       <c r="B10" s="2">
@@ -2332,16 +2117,9 @@
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+      <c r="A11">
         <v>16</v>
       </c>
       <c r="B11" s="2">
@@ -2350,16 +2128,9 @@
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+      <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" s="2">
@@ -2368,16 +2139,9 @@
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+      <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" s="2">
@@ -2386,16 +2150,9 @@
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+      <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" s="2">
@@ -2404,16 +2161,9 @@
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+      <c r="A15">
         <v>6</v>
       </c>
       <c r="B15" s="2">
@@ -2422,16 +2172,9 @@
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+      <c r="A16">
         <v>6</v>
       </c>
       <c r="B16" s="2">
@@ -2440,16 +2183,9 @@
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>6</v>
       </c>
       <c r="B17" s="2">
@@ -2458,16 +2194,9 @@
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="2">
@@ -2476,16 +2205,9 @@
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" s="2">
@@ -2494,16 +2216,9 @@
       <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" s="2">
@@ -2512,16 +2227,9 @@
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>16</v>
       </c>
       <c r="B21" s="2">
@@ -2530,16 +2238,9 @@
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>16</v>
       </c>
       <c r="B22" s="2">
@@ -2548,13 +2249,6 @@
       <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>